<commit_message>
Actualizacion Base de Datos
</commit_message>
<xml_diff>
--- a/ProductosBDD.xlsx
+++ b/ProductosBDD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\OneDrive\Escritorio\Multiservicios Brufas\Multiservicios_Brufas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6A5199-F40E-407F-9C9E-80BB7E6C06E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66195487-1A12-4373-913B-5756FA488861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="265">
   <si>
     <t>CATEGORIA</t>
   </si>
@@ -681,12 +681,6 @@
     <t>PLUMONES JUNIOR STANDFORD 12UND</t>
   </si>
   <si>
-    <t>LAPICEROS DE COLORES MEDIANOS OVAL 12UND</t>
-  </si>
-  <si>
-    <t>LAPICEROS DE COLORES GRANDES OVAL 12UND</t>
-  </si>
-  <si>
     <t>LAPIZ GRAFITO ARTESCO 1UND</t>
   </si>
   <si>
@@ -712,6 +706,120 @@
   </si>
   <si>
     <t>LAPICEROS ESCARCHADOS NAYRAS 12UND</t>
+  </si>
+  <si>
+    <t>CERVEZA BOTELLA</t>
+  </si>
+  <si>
+    <t>CORONITA 210ML</t>
+  </si>
+  <si>
+    <t>CORONA 330ML</t>
+  </si>
+  <si>
+    <t>CORONA SIX PACK BOTELLA 330ML</t>
+  </si>
+  <si>
+    <t>CORONITA SIX PACK BOTELLA 210ML</t>
+  </si>
+  <si>
+    <t>CREAM TABACCO 500 PUFFS</t>
+  </si>
+  <si>
+    <t>GRAPE ICE 500 PUFFS</t>
+  </si>
+  <si>
+    <t>AGUAS</t>
+  </si>
+  <si>
+    <t>AGUA SAN LUIS SIN GAS 3L</t>
+  </si>
+  <si>
+    <t>AGUA SAN LUIS CON GAS 3L</t>
+  </si>
+  <si>
+    <t>AGUA SAN LUIS SIN GAS 1L</t>
+  </si>
+  <si>
+    <t>AGUA SAN LUIS SIN GAS 500ML</t>
+  </si>
+  <si>
+    <t>AGUA SAN LUIS CON GAS 500ML</t>
+  </si>
+  <si>
+    <t>AGUA CIELO SIN GAS 1L</t>
+  </si>
+  <si>
+    <t>AGUA CIELO SIN GAS 500ML</t>
+  </si>
+  <si>
+    <t>AGUA CIELO CON GAS 500ML</t>
+  </si>
+  <si>
+    <t>ENERGIZANTES</t>
+  </si>
+  <si>
+    <t>MONSTER ENERGY 473ML</t>
+  </si>
+  <si>
+    <t>RED BULL 355ML</t>
+  </si>
+  <si>
+    <t>ENERGIZANTE VOLT 300ML</t>
+  </si>
+  <si>
+    <t>JUGOS</t>
+  </si>
+  <si>
+    <t>FRUGOS DEL VALLE NARANJA 3L</t>
+  </si>
+  <si>
+    <t>FRUGOS DEL VALLE NARANJA 1.5L</t>
+  </si>
+  <si>
+    <t>JUGO DE NARANJA GLORIA 1L</t>
+  </si>
+  <si>
+    <t>FRUGOS DEL VALLE NARANJA 500ML</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JUGO CIFRUT NARANJA 500ML </t>
+  </si>
+  <si>
+    <t>REHIDRATANTES</t>
+  </si>
+  <si>
+    <t>POWERADE MORA 1.5L</t>
+  </si>
+  <si>
+    <t>POWERADE MORA 1L</t>
+  </si>
+  <si>
+    <t>SPORADE TROPICAL 1.5L</t>
+  </si>
+  <si>
+    <t>SPORADE TROPICAL 500ML</t>
+  </si>
+  <si>
+    <t>POWERADE MORA 500ML</t>
+  </si>
+  <si>
+    <t>GATORADE TROPICAL 500ML</t>
+  </si>
+  <si>
+    <t>ESTUCHE DE REGLAS</t>
+  </si>
+  <si>
+    <t>CINTA SCOTCH DURAFAN</t>
+  </si>
+  <si>
+    <t>LÁPICES DE COLORES GRANDES OVAL 12UND</t>
+  </si>
+  <si>
+    <t>LÁPICES DE COLORES MEDIANOS OVAL 12UND</t>
+  </si>
+  <si>
+    <t>LAPICERO CLASICO OVAL</t>
   </si>
 </sst>
 </file>
@@ -1029,10 +1137,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C207"/>
+  <dimension ref="A1:C238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="C134" sqref="C134"/>
+    <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
+      <selection activeCell="D207" sqref="D207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1132,24 +1240,24 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>227</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>228</v>
       </c>
       <c r="C9">
-        <v>25</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>227</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>229</v>
       </c>
       <c r="C10">
-        <v>17</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -1157,7 +1265,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C11">
         <v>25</v>
@@ -1168,10 +1276,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C12">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -1179,10 +1287,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C13">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -1190,10 +1298,10 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C14">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -1201,54 +1309,54 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C15">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C16">
-        <v>63</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C17">
-        <v>65</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>231</v>
       </c>
       <c r="C18">
-        <v>69</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>230</v>
       </c>
       <c r="C19">
-        <v>72</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -1256,10 +1364,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C20">
-        <v>74</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -1267,10 +1375,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C21">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -1278,10 +1386,10 @@
         <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C22">
-        <v>40</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -1289,10 +1397,10 @@
         <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C23">
-        <v>60</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -1300,10 +1408,10 @@
         <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C24">
-        <v>60</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
@@ -1311,54 +1419,54 @@
         <v>19</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C25">
-        <v>60</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C26">
-        <v>6</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C27">
-        <v>7</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C28">
-        <v>7</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B29" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C29">
-        <v>7</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
@@ -1366,54 +1474,54 @@
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C30">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C31">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C32">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B33" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C33">
-        <v>8.5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C34">
-        <v>8.5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
@@ -1421,10 +1529,10 @@
         <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C35">
-        <v>6.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
@@ -1432,10 +1540,10 @@
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C36">
-        <v>6.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
@@ -1443,10 +1551,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C37">
-        <v>5.5</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
@@ -1454,10 +1562,10 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C38">
-        <v>3.8</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
@@ -1465,10 +1573,10 @@
         <v>36</v>
       </c>
       <c r="B39" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C39">
-        <v>3.8</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
@@ -1476,10 +1584,10 @@
         <v>36</v>
       </c>
       <c r="B40" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C40">
-        <v>2.8</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
@@ -1487,10 +1595,10 @@
         <v>36</v>
       </c>
       <c r="B41" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C41">
-        <v>2.8</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
@@ -1498,10 +1606,10 @@
         <v>36</v>
       </c>
       <c r="B42" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C42">
-        <v>1.5</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
@@ -1509,10 +1617,10 @@
         <v>36</v>
       </c>
       <c r="B43" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C43">
-        <v>1.5</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
@@ -1520,10 +1628,10 @@
         <v>36</v>
       </c>
       <c r="B44" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C44">
-        <v>1</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
@@ -1531,10 +1639,10 @@
         <v>36</v>
       </c>
       <c r="B45" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C45">
-        <v>1</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
@@ -1542,10 +1650,10 @@
         <v>36</v>
       </c>
       <c r="B46" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C46">
-        <v>8</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
@@ -1553,10 +1661,10 @@
         <v>36</v>
       </c>
       <c r="B47" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C47">
-        <v>8</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
@@ -1564,10 +1672,10 @@
         <v>36</v>
       </c>
       <c r="B48" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C48">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
@@ -1575,10 +1683,10 @@
         <v>36</v>
       </c>
       <c r="B49" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C49">
-        <v>5.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
@@ -1586,10 +1694,10 @@
         <v>36</v>
       </c>
       <c r="B50" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C50">
-        <v>4.5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
@@ -1597,10 +1705,10 @@
         <v>36</v>
       </c>
       <c r="B51" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C51">
-        <v>3.5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
@@ -1608,10 +1716,10 @@
         <v>36</v>
       </c>
       <c r="B52" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C52">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
@@ -1619,10 +1727,10 @@
         <v>36</v>
       </c>
       <c r="B53" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C53">
-        <v>1.5</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
@@ -1630,10 +1738,10 @@
         <v>36</v>
       </c>
       <c r="B54" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C54">
-        <v>1.5</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
@@ -1641,10 +1749,10 @@
         <v>36</v>
       </c>
       <c r="B55" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C55">
-        <v>1</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
@@ -1652,10 +1760,10 @@
         <v>36</v>
       </c>
       <c r="B56" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C56">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
@@ -1663,18 +1771,18 @@
         <v>36</v>
       </c>
       <c r="B57" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C57">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="B58" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C58">
         <v>1.5</v>
@@ -1682,109 +1790,109 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="B59" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C59">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="B60" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C60">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="B61" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C61">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>64</v>
+        <v>234</v>
       </c>
       <c r="B62" t="s">
-        <v>69</v>
+        <v>235</v>
       </c>
       <c r="C62">
-        <v>1.5</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>64</v>
+        <v>234</v>
       </c>
       <c r="B63" t="s">
-        <v>70</v>
+        <v>236</v>
       </c>
       <c r="C63">
-        <v>1.5</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>64</v>
+        <v>234</v>
       </c>
       <c r="B64" t="s">
-        <v>71</v>
+        <v>237</v>
       </c>
       <c r="C64">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>64</v>
+        <v>234</v>
       </c>
       <c r="B65" t="s">
-        <v>72</v>
+        <v>238</v>
       </c>
       <c r="C65">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>64</v>
+        <v>234</v>
       </c>
       <c r="B66" t="s">
-        <v>73</v>
+        <v>239</v>
       </c>
       <c r="C66">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>64</v>
+        <v>234</v>
       </c>
       <c r="B67" t="s">
-        <v>74</v>
+        <v>240</v>
       </c>
       <c r="C67">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>64</v>
+        <v>234</v>
       </c>
       <c r="B68" t="s">
-        <v>75</v>
+        <v>241</v>
       </c>
       <c r="C68">
         <v>1</v>
@@ -1792,10 +1900,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>64</v>
+        <v>234</v>
       </c>
       <c r="B69" t="s">
-        <v>76</v>
+        <v>242</v>
       </c>
       <c r="C69">
         <v>1</v>
@@ -1803,87 +1911,87 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>64</v>
+        <v>243</v>
       </c>
       <c r="B70" t="s">
-        <v>77</v>
+        <v>244</v>
       </c>
       <c r="C70">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>64</v>
+        <v>243</v>
       </c>
       <c r="B71" t="s">
-        <v>78</v>
+        <v>245</v>
       </c>
       <c r="C71">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>64</v>
+        <v>243</v>
       </c>
       <c r="B72" t="s">
-        <v>79</v>
+        <v>246</v>
       </c>
       <c r="C72">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>64</v>
+        <v>247</v>
       </c>
       <c r="B73" t="s">
-        <v>80</v>
+        <v>248</v>
       </c>
       <c r="C73">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>64</v>
+        <v>247</v>
       </c>
       <c r="B74" t="s">
-        <v>81</v>
+        <v>249</v>
       </c>
       <c r="C74">
-        <v>1</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>64</v>
+        <v>247</v>
       </c>
       <c r="B75" t="s">
-        <v>82</v>
+        <v>250</v>
       </c>
       <c r="C75">
-        <v>1</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>64</v>
+        <v>247</v>
       </c>
       <c r="B76" t="s">
-        <v>83</v>
+        <v>251</v>
       </c>
       <c r="C76">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>64</v>
+        <v>247</v>
       </c>
       <c r="B77" t="s">
-        <v>84</v>
+        <v>252</v>
       </c>
       <c r="C77">
         <v>1</v>
@@ -1891,68 +1999,68 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>64</v>
+        <v>253</v>
       </c>
       <c r="B78" t="s">
-        <v>85</v>
+        <v>254</v>
       </c>
       <c r="C78">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>64</v>
+        <v>253</v>
       </c>
       <c r="B79" t="s">
-        <v>86</v>
+        <v>255</v>
       </c>
       <c r="C79">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>64</v>
+        <v>253</v>
       </c>
       <c r="B80" t="s">
-        <v>87</v>
+        <v>256</v>
       </c>
       <c r="C80">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>64</v>
+        <v>253</v>
       </c>
       <c r="B81" t="s">
-        <v>88</v>
+        <v>257</v>
       </c>
       <c r="C81">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>64</v>
+        <v>253</v>
       </c>
       <c r="B82" t="s">
-        <v>89</v>
+        <v>258</v>
       </c>
       <c r="C82">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>64</v>
+        <v>253</v>
       </c>
       <c r="B83" t="s">
-        <v>90</v>
+        <v>259</v>
       </c>
       <c r="C83">
-        <v>1</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
@@ -1960,10 +2068,10 @@
         <v>64</v>
       </c>
       <c r="B84" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="C84">
-        <v>0.7</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
@@ -1971,7 +2079,7 @@
         <v>64</v>
       </c>
       <c r="B85" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="C85">
         <v>1.5</v>
@@ -1982,10 +2090,10 @@
         <v>64</v>
       </c>
       <c r="B86" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
       <c r="C86">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
@@ -1993,10 +2101,10 @@
         <v>64</v>
       </c>
       <c r="B87" t="s">
-        <v>94</v>
+        <v>68</v>
       </c>
       <c r="C87">
-        <v>2.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
@@ -2004,10 +2112,10 @@
         <v>64</v>
       </c>
       <c r="B88" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="C88">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
@@ -2015,10 +2123,10 @@
         <v>64</v>
       </c>
       <c r="B89" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="C89">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
@@ -2026,18 +2134,18 @@
         <v>64</v>
       </c>
       <c r="B90" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="C90">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>98</v>
+        <v>64</v>
       </c>
       <c r="B91" t="s">
-        <v>99</v>
+        <v>72</v>
       </c>
       <c r="C91">
         <v>1</v>
@@ -2045,21 +2153,21 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>98</v>
+        <v>64</v>
       </c>
       <c r="B92" t="s">
-        <v>100</v>
+        <v>73</v>
       </c>
       <c r="C92">
-        <v>1.4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>98</v>
+        <v>64</v>
       </c>
       <c r="B93" t="s">
-        <v>101</v>
+        <v>74</v>
       </c>
       <c r="C93">
         <v>1</v>
@@ -2067,10 +2175,10 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>98</v>
+        <v>64</v>
       </c>
       <c r="B94" t="s">
-        <v>102</v>
+        <v>75</v>
       </c>
       <c r="C94">
         <v>1</v>
@@ -2078,10 +2186,10 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>98</v>
+        <v>64</v>
       </c>
       <c r="B95" t="s">
-        <v>103</v>
+        <v>76</v>
       </c>
       <c r="C95">
         <v>1</v>
@@ -2089,10 +2197,10 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>98</v>
+        <v>64</v>
       </c>
       <c r="B96" t="s">
-        <v>104</v>
+        <v>77</v>
       </c>
       <c r="C96">
         <v>1</v>
@@ -2100,10 +2208,10 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>98</v>
+        <v>64</v>
       </c>
       <c r="B97" t="s">
-        <v>105</v>
+        <v>78</v>
       </c>
       <c r="C97">
         <v>1</v>
@@ -2111,219 +2219,219 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>98</v>
+        <v>64</v>
       </c>
       <c r="B98" t="s">
-        <v>106</v>
+        <v>79</v>
       </c>
       <c r="C98">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>98</v>
+        <v>64</v>
       </c>
       <c r="B99" t="s">
-        <v>107</v>
+        <v>80</v>
       </c>
       <c r="C99">
-        <v>8.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>98</v>
+        <v>64</v>
       </c>
       <c r="B100" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="C100">
-        <v>8.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>98</v>
+        <v>64</v>
       </c>
       <c r="B101" t="s">
-        <v>109</v>
+        <v>82</v>
       </c>
       <c r="C101">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>98</v>
+        <v>64</v>
       </c>
       <c r="B102" t="s">
-        <v>110</v>
+        <v>83</v>
       </c>
       <c r="C102">
-        <v>5.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>98</v>
+        <v>64</v>
       </c>
       <c r="B103" t="s">
-        <v>111</v>
+        <v>84</v>
       </c>
       <c r="C103">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>112</v>
+        <v>64</v>
       </c>
       <c r="B104" t="s">
-        <v>113</v>
+        <v>85</v>
       </c>
       <c r="C104">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>112</v>
+        <v>64</v>
       </c>
       <c r="B105" t="s">
-        <v>114</v>
+        <v>86</v>
       </c>
       <c r="C105">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>112</v>
+        <v>64</v>
       </c>
       <c r="B106" t="s">
-        <v>115</v>
+        <v>87</v>
       </c>
       <c r="C106">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>112</v>
+        <v>64</v>
       </c>
       <c r="B107" t="s">
-        <v>116</v>
+        <v>88</v>
       </c>
       <c r="C107">
-        <v>1.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>112</v>
+        <v>64</v>
       </c>
       <c r="B108" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="C108">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>112</v>
+        <v>64</v>
       </c>
       <c r="B109" t="s">
-        <v>118</v>
+        <v>90</v>
       </c>
       <c r="C109">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>119</v>
+        <v>64</v>
       </c>
       <c r="B110" t="s">
-        <v>120</v>
+        <v>91</v>
       </c>
       <c r="C110">
-        <v>1.2</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>119</v>
+        <v>64</v>
       </c>
       <c r="B111" t="s">
-        <v>121</v>
+        <v>92</v>
       </c>
       <c r="C111">
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>119</v>
+        <v>64</v>
       </c>
       <c r="B112" t="s">
-        <v>122</v>
+        <v>93</v>
       </c>
       <c r="C112">
-        <v>3</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>119</v>
+        <v>64</v>
       </c>
       <c r="B113" t="s">
-        <v>123</v>
+        <v>94</v>
       </c>
       <c r="C113">
-        <v>3</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>119</v>
+        <v>64</v>
       </c>
       <c r="B114" t="s">
-        <v>124</v>
+        <v>95</v>
       </c>
       <c r="C114">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>119</v>
+        <v>64</v>
       </c>
       <c r="B115" t="s">
-        <v>125</v>
+        <v>96</v>
       </c>
       <c r="C115">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>119</v>
+        <v>64</v>
       </c>
       <c r="B116" t="s">
-        <v>126</v>
+        <v>97</v>
       </c>
       <c r="C116">
-        <v>1.5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="B117" t="s">
-        <v>127</v>
+        <v>99</v>
       </c>
       <c r="C117">
         <v>1</v>
@@ -2331,21 +2439,21 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="B118" t="s">
-        <v>128</v>
+        <v>100</v>
       </c>
       <c r="C118">
-        <v>0.5</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>129</v>
+        <v>98</v>
       </c>
       <c r="B119" t="s">
-        <v>130</v>
+        <v>101</v>
       </c>
       <c r="C119">
         <v>1</v>
@@ -2353,916 +2461,1311 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>129</v>
+        <v>98</v>
       </c>
       <c r="B120" t="s">
-        <v>131</v>
+        <v>102</v>
       </c>
       <c r="C120">
-        <v>1.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>129</v>
+        <v>98</v>
       </c>
       <c r="B121" t="s">
-        <v>132</v>
+        <v>103</v>
       </c>
       <c r="C121">
-        <v>1.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>129</v>
+        <v>98</v>
       </c>
       <c r="B122" t="s">
-        <v>133</v>
+        <v>104</v>
       </c>
       <c r="C122">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>129</v>
+        <v>98</v>
       </c>
       <c r="B123" t="s">
-        <v>134</v>
+        <v>105</v>
       </c>
       <c r="C123">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>129</v>
+        <v>98</v>
       </c>
       <c r="B124" t="s">
-        <v>135</v>
+        <v>106</v>
       </c>
       <c r="C124">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>129</v>
+        <v>98</v>
       </c>
       <c r="B125" t="s">
-        <v>136</v>
+        <v>107</v>
       </c>
       <c r="C125">
-        <v>12</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>129</v>
+        <v>98</v>
       </c>
       <c r="B126" t="s">
-        <v>137</v>
+        <v>108</v>
       </c>
       <c r="C126">
-        <v>8</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>138</v>
+        <v>98</v>
       </c>
       <c r="B127" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
       <c r="C127">
-        <v>20</v>
+        <v>7</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>138</v>
+        <v>98</v>
       </c>
       <c r="B128" t="s">
-        <v>140</v>
+        <v>110</v>
       </c>
       <c r="C128">
-        <v>35</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>138</v>
+        <v>98</v>
       </c>
       <c r="B129" t="s">
-        <v>141</v>
+        <v>111</v>
       </c>
       <c r="C129">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>138</v>
+        <v>112</v>
       </c>
       <c r="B130" t="s">
-        <v>142</v>
+        <v>113</v>
       </c>
       <c r="C130">
-        <v>35</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>138</v>
+        <v>112</v>
       </c>
       <c r="B131" t="s">
-        <v>143</v>
+        <v>114</v>
       </c>
       <c r="C131">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>138</v>
+        <v>112</v>
       </c>
       <c r="B132" t="s">
-        <v>144</v>
+        <v>115</v>
       </c>
       <c r="C132">
-        <v>35</v>
+        <v>2</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>138</v>
+        <v>112</v>
       </c>
       <c r="B133" t="s">
-        <v>145</v>
+        <v>116</v>
       </c>
       <c r="C133">
-        <v>20</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>138</v>
+        <v>112</v>
       </c>
       <c r="B134" t="s">
-        <v>146</v>
+        <v>117</v>
       </c>
       <c r="C134">
-        <v>35</v>
+        <v>13</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>147</v>
+        <v>112</v>
       </c>
       <c r="B135" t="s">
-        <v>148</v>
+        <v>118</v>
       </c>
       <c r="C135">
-        <v>37</v>
+        <v>2</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>147</v>
+        <v>119</v>
       </c>
       <c r="B136" t="s">
-        <v>149</v>
+        <v>120</v>
       </c>
       <c r="C136">
-        <v>46.5</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>147</v>
+        <v>119</v>
       </c>
       <c r="B137" t="s">
-        <v>150</v>
+        <v>121</v>
       </c>
       <c r="C137">
-        <v>57</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>147</v>
+        <v>119</v>
       </c>
       <c r="B138" t="s">
-        <v>151</v>
+        <v>122</v>
       </c>
       <c r="C138">
-        <v>36</v>
+        <v>3</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>147</v>
+        <v>119</v>
       </c>
       <c r="B139" t="s">
-        <v>152</v>
+        <v>123</v>
       </c>
       <c r="C139">
-        <v>46</v>
+        <v>3</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>147</v>
+        <v>119</v>
       </c>
       <c r="B140" t="s">
-        <v>153</v>
+        <v>124</v>
       </c>
       <c r="C140">
-        <v>33</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>147</v>
+        <v>119</v>
       </c>
       <c r="B141" t="s">
-        <v>154</v>
+        <v>125</v>
       </c>
       <c r="C141">
-        <v>41</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>147</v>
+        <v>119</v>
       </c>
       <c r="B142" t="s">
-        <v>155</v>
+        <v>126</v>
       </c>
       <c r="C142">
-        <v>60</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>147</v>
+        <v>119</v>
       </c>
       <c r="B143" t="s">
-        <v>156</v>
+        <v>127</v>
       </c>
       <c r="C143">
-        <v>17</v>
+        <v>1</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>147</v>
+        <v>119</v>
       </c>
       <c r="B144" t="s">
-        <v>157</v>
+        <v>128</v>
       </c>
       <c r="C144">
-        <v>30</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="B145" t="s">
-        <v>158</v>
+        <v>130</v>
       </c>
       <c r="C145">
-        <v>30</v>
+        <v>1</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="B146" t="s">
-        <v>159</v>
+        <v>131</v>
       </c>
       <c r="C146">
-        <v>38</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="B147" t="s">
-        <v>160</v>
+        <v>132</v>
       </c>
       <c r="C147">
-        <v>29</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="B148" t="s">
-        <v>161</v>
+        <v>133</v>
       </c>
       <c r="C148">
-        <v>29</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="B149" t="s">
-        <v>162</v>
+        <v>134</v>
       </c>
       <c r="C149">
-        <v>29</v>
+        <v>8</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>163</v>
+        <v>129</v>
       </c>
       <c r="B150" t="s">
-        <v>164</v>
+        <v>135</v>
       </c>
       <c r="C150">
-        <v>55</v>
+        <v>12</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>163</v>
+        <v>129</v>
       </c>
       <c r="B151" t="s">
-        <v>165</v>
+        <v>136</v>
       </c>
       <c r="C151">
-        <v>47</v>
+        <v>12</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>163</v>
+        <v>129</v>
       </c>
       <c r="B152" t="s">
-        <v>166</v>
+        <v>137</v>
       </c>
       <c r="C152">
-        <v>56</v>
+        <v>8</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>163</v>
+        <v>138</v>
       </c>
       <c r="B153" t="s">
-        <v>167</v>
+        <v>139</v>
       </c>
       <c r="C153">
-        <v>48</v>
+        <v>20</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>163</v>
+        <v>138</v>
       </c>
       <c r="B154" t="s">
-        <v>168</v>
+        <v>140</v>
       </c>
       <c r="C154">
-        <v>75</v>
+        <v>35</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>163</v>
+        <v>138</v>
       </c>
       <c r="B155" t="s">
-        <v>169</v>
+        <v>141</v>
       </c>
       <c r="C155">
-        <v>65</v>
+        <v>20</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>163</v>
+        <v>138</v>
       </c>
       <c r="B156" t="s">
-        <v>170</v>
+        <v>142</v>
       </c>
       <c r="C156">
-        <v>54</v>
+        <v>35</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>171</v>
+        <v>138</v>
       </c>
       <c r="B157" t="s">
-        <v>172</v>
+        <v>143</v>
       </c>
       <c r="C157">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>171</v>
+        <v>138</v>
       </c>
       <c r="B158" t="s">
-        <v>173</v>
+        <v>144</v>
       </c>
       <c r="C158">
-        <v>53</v>
+        <v>35</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>171</v>
+        <v>138</v>
       </c>
       <c r="B159" t="s">
-        <v>174</v>
+        <v>145</v>
       </c>
       <c r="C159">
-        <v>55</v>
+        <v>20</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>171</v>
+        <v>138</v>
       </c>
       <c r="B160" t="s">
-        <v>175</v>
+        <v>146</v>
       </c>
       <c r="C160">
-        <v>100</v>
+        <v>35</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>171</v>
+        <v>138</v>
       </c>
       <c r="B161" t="s">
-        <v>176</v>
+        <v>233</v>
       </c>
       <c r="C161">
-        <v>110</v>
+        <v>20</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>171</v>
+        <v>138</v>
       </c>
       <c r="B162" t="s">
-        <v>177</v>
+        <v>232</v>
       </c>
       <c r="C162">
-        <v>55</v>
+        <v>15</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
       <c r="B163" t="s">
-        <v>178</v>
+        <v>148</v>
       </c>
       <c r="C163">
-        <v>125</v>
+        <v>37</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
       <c r="B164" t="s">
-        <v>179</v>
+        <v>149</v>
       </c>
       <c r="C164">
-        <v>150</v>
+        <v>46.5</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
       <c r="B165" t="s">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="C165">
-        <v>245</v>
+        <v>57</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>181</v>
+        <v>147</v>
       </c>
       <c r="B166" t="s">
-        <v>182</v>
+        <v>151</v>
       </c>
       <c r="C166">
-        <v>32.5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>181</v>
+        <v>147</v>
       </c>
       <c r="B167" t="s">
-        <v>183</v>
+        <v>152</v>
       </c>
       <c r="C167">
-        <v>32.5</v>
+        <v>46</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>184</v>
+        <v>147</v>
       </c>
       <c r="B168" t="s">
-        <v>185</v>
+        <v>153</v>
       </c>
       <c r="C168">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>184</v>
+        <v>147</v>
       </c>
       <c r="B169" t="s">
-        <v>186</v>
+        <v>154</v>
       </c>
       <c r="C169">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>184</v>
+        <v>147</v>
       </c>
       <c r="B170" t="s">
-        <v>187</v>
+        <v>155</v>
       </c>
       <c r="C170">
-        <v>28</v>
+        <v>60</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>188</v>
+        <v>147</v>
       </c>
       <c r="B171" t="s">
-        <v>189</v>
+        <v>156</v>
       </c>
       <c r="C171">
-        <v>18.5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>188</v>
+        <v>147</v>
       </c>
       <c r="B172" t="s">
-        <v>190</v>
+        <v>157</v>
       </c>
       <c r="C172">
-        <v>18.5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>188</v>
+        <v>147</v>
       </c>
       <c r="B173" t="s">
-        <v>191</v>
+        <v>158</v>
       </c>
       <c r="C173">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>192</v>
+        <v>147</v>
       </c>
       <c r="B174" t="s">
-        <v>193</v>
+        <v>159</v>
       </c>
       <c r="C174">
-        <v>75</v>
+        <v>38</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>192</v>
+        <v>147</v>
       </c>
       <c r="B175" t="s">
-        <v>194</v>
+        <v>160</v>
       </c>
       <c r="C175">
-        <v>78</v>
+        <v>29</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>192</v>
+        <v>147</v>
       </c>
       <c r="B176" t="s">
-        <v>195</v>
+        <v>161</v>
       </c>
       <c r="C176">
-        <v>100</v>
+        <v>29</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>192</v>
+        <v>147</v>
       </c>
       <c r="B177" t="s">
-        <v>196</v>
+        <v>162</v>
       </c>
       <c r="C177">
-        <v>10</v>
+        <v>29</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>192</v>
+        <v>163</v>
       </c>
       <c r="B178" t="s">
-        <v>197</v>
+        <v>164</v>
       </c>
       <c r="C178">
-        <v>6</v>
+        <v>55</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>192</v>
+        <v>163</v>
       </c>
       <c r="B179" t="s">
-        <v>198</v>
+        <v>165</v>
+      </c>
+      <c r="C179">
+        <v>47</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>192</v>
+        <v>163</v>
       </c>
       <c r="B180" t="s">
-        <v>199</v>
+        <v>166</v>
       </c>
       <c r="C180">
-        <v>5</v>
+        <v>56</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>192</v>
+        <v>163</v>
       </c>
       <c r="B181" t="s">
-        <v>200</v>
+        <v>167</v>
       </c>
       <c r="C181">
-        <v>5</v>
+        <v>48</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>201</v>
+        <v>163</v>
       </c>
       <c r="B182" t="s">
-        <v>202</v>
+        <v>168</v>
       </c>
       <c r="C182">
-        <v>4</v>
+        <v>75</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>201</v>
+        <v>163</v>
       </c>
       <c r="B183" t="s">
-        <v>203</v>
+        <v>169</v>
       </c>
       <c r="C183">
-        <v>3</v>
+        <v>65</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>201</v>
+        <v>163</v>
       </c>
       <c r="B184" t="s">
-        <v>204</v>
+        <v>170</v>
       </c>
       <c r="C184">
-        <v>5</v>
+        <v>54</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>201</v>
+        <v>171</v>
       </c>
       <c r="B185" t="s">
-        <v>205</v>
+        <v>172</v>
       </c>
       <c r="C185">
-        <v>5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>206</v>
+        <v>171</v>
       </c>
       <c r="B186" t="s">
-        <v>207</v>
+        <v>173</v>
       </c>
       <c r="C186">
-        <v>5.5</v>
+        <v>53</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>206</v>
+        <v>171</v>
       </c>
       <c r="B187" t="s">
-        <v>208</v>
+        <v>174</v>
       </c>
       <c r="C187">
-        <v>5.5</v>
+        <v>55</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>206</v>
+        <v>171</v>
       </c>
       <c r="B188" t="s">
-        <v>209</v>
+        <v>175</v>
+      </c>
+      <c r="C188">
+        <v>100</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>206</v>
+        <v>171</v>
       </c>
       <c r="B189" t="s">
-        <v>210</v>
+        <v>176</v>
+      </c>
+      <c r="C189">
+        <v>110</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>206</v>
+        <v>171</v>
       </c>
       <c r="B190" t="s">
-        <v>211</v>
+        <v>177</v>
+      </c>
+      <c r="C190">
+        <v>55</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>206</v>
+        <v>171</v>
       </c>
       <c r="B191" t="s">
-        <v>212</v>
+        <v>178</v>
+      </c>
+      <c r="C191">
+        <v>125</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>206</v>
+        <v>171</v>
       </c>
       <c r="B192" t="s">
-        <v>213</v>
+        <v>179</v>
+      </c>
+      <c r="C192">
+        <v>150</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>206</v>
+        <v>171</v>
       </c>
       <c r="B193" t="s">
-        <v>214</v>
+        <v>180</v>
+      </c>
+      <c r="C193">
+        <v>245</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>206</v>
+        <v>181</v>
       </c>
       <c r="B194" t="s">
-        <v>215</v>
+        <v>182</v>
+      </c>
+      <c r="C194">
+        <v>32.5</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>206</v>
+        <v>181</v>
       </c>
       <c r="B195" t="s">
-        <v>216</v>
+        <v>183</v>
+      </c>
+      <c r="C195">
+        <v>32.5</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>206</v>
+        <v>184</v>
       </c>
       <c r="B196" t="s">
-        <v>217</v>
+        <v>185</v>
+      </c>
+      <c r="C196">
+        <v>26</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>206</v>
+        <v>184</v>
       </c>
       <c r="B197" t="s">
-        <v>218</v>
+        <v>186</v>
+      </c>
+      <c r="C197">
+        <v>51</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>206</v>
+        <v>184</v>
       </c>
       <c r="B198" t="s">
-        <v>219</v>
+        <v>187</v>
+      </c>
+      <c r="C198">
+        <v>28</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>206</v>
+        <v>188</v>
       </c>
       <c r="B199" t="s">
-        <v>220</v>
+        <v>189</v>
       </c>
       <c r="C199">
-        <v>0.6</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>206</v>
+        <v>188</v>
       </c>
       <c r="B200" t="s">
-        <v>221</v>
+        <v>190</v>
       </c>
       <c r="C200">
-        <v>2.5</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
-        <v>206</v>
+        <v>188</v>
       </c>
       <c r="B201" t="s">
-        <v>222</v>
+        <v>191</v>
+      </c>
+      <c r="C201">
+        <v>15</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="B202" t="s">
-        <v>223</v>
+        <v>193</v>
+      </c>
+      <c r="C202">
+        <v>75</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="B203" t="s">
-        <v>224</v>
+        <v>194</v>
+      </c>
+      <c r="C203">
+        <v>78</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="B204" t="s">
-        <v>225</v>
+        <v>195</v>
+      </c>
+      <c r="C204">
+        <v>100</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="B205" t="s">
-        <v>226</v>
+        <v>196</v>
+      </c>
+      <c r="C205">
+        <v>10</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="B206" t="s">
-        <v>227</v>
+        <v>197</v>
+      </c>
+      <c r="C206">
+        <v>6</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
+        <v>192</v>
+      </c>
+      <c r="B207" t="s">
+        <v>198</v>
+      </c>
+      <c r="C207">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A208" t="s">
+        <v>192</v>
+      </c>
+      <c r="B208" t="s">
+        <v>199</v>
+      </c>
+      <c r="C208">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A209" t="s">
+        <v>192</v>
+      </c>
+      <c r="B209" t="s">
+        <v>200</v>
+      </c>
+      <c r="C209">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A210" t="s">
+        <v>201</v>
+      </c>
+      <c r="B210" t="s">
+        <v>202</v>
+      </c>
+      <c r="C210">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A211" t="s">
+        <v>201</v>
+      </c>
+      <c r="B211" t="s">
+        <v>203</v>
+      </c>
+      <c r="C211">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A212" t="s">
+        <v>201</v>
+      </c>
+      <c r="B212" t="s">
+        <v>204</v>
+      </c>
+      <c r="C212">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A213" t="s">
+        <v>201</v>
+      </c>
+      <c r="B213" t="s">
+        <v>205</v>
+      </c>
+      <c r="C213">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A214" t="s">
         <v>206</v>
       </c>
-      <c r="B207" t="s">
-        <v>228</v>
-      </c>
-      <c r="C207">
+      <c r="B214" t="s">
+        <v>207</v>
+      </c>
+      <c r="C214">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A215" t="s">
+        <v>206</v>
+      </c>
+      <c r="B215" t="s">
+        <v>208</v>
+      </c>
+      <c r="C215">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A216" t="s">
+        <v>206</v>
+      </c>
+      <c r="B216" t="s">
+        <v>209</v>
+      </c>
+      <c r="C216">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A217" t="s">
+        <v>206</v>
+      </c>
+      <c r="B217" t="s">
+        <v>210</v>
+      </c>
+      <c r="C217">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A218" t="s">
+        <v>206</v>
+      </c>
+      <c r="B218" t="s">
+        <v>211</v>
+      </c>
+      <c r="C218">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A219" t="s">
+        <v>206</v>
+      </c>
+      <c r="B219" t="s">
+        <v>212</v>
+      </c>
+      <c r="C219">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A220" t="s">
+        <v>206</v>
+      </c>
+      <c r="B220" t="s">
+        <v>213</v>
+      </c>
+      <c r="C220">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A221" t="s">
+        <v>206</v>
+      </c>
+      <c r="B221" t="s">
+        <v>214</v>
+      </c>
+      <c r="C221">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A222" t="s">
+        <v>206</v>
+      </c>
+      <c r="B222" t="s">
+        <v>215</v>
+      </c>
+      <c r="C222">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A223" t="s">
+        <v>206</v>
+      </c>
+      <c r="B223" t="s">
+        <v>216</v>
+      </c>
+      <c r="C223">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A224" t="s">
+        <v>206</v>
+      </c>
+      <c r="B224" t="s">
+        <v>217</v>
+      </c>
+      <c r="C224">
         <v>7</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A225" t="s">
+        <v>206</v>
+      </c>
+      <c r="B225" t="s">
+        <v>263</v>
+      </c>
+      <c r="C225">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A226" t="s">
+        <v>206</v>
+      </c>
+      <c r="B226" t="s">
+        <v>262</v>
+      </c>
+      <c r="C226">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A227" t="s">
+        <v>206</v>
+      </c>
+      <c r="B227" t="s">
+        <v>218</v>
+      </c>
+      <c r="C227">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A228" t="s">
+        <v>206</v>
+      </c>
+      <c r="B228" t="s">
+        <v>219</v>
+      </c>
+      <c r="C228">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A229" t="s">
+        <v>206</v>
+      </c>
+      <c r="B229" t="s">
+        <v>220</v>
+      </c>
+      <c r="C229">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A230" t="s">
+        <v>206</v>
+      </c>
+      <c r="B230" t="s">
+        <v>221</v>
+      </c>
+      <c r="C230">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A231" t="s">
+        <v>206</v>
+      </c>
+      <c r="B231" t="s">
+        <v>222</v>
+      </c>
+      <c r="C231">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A232" t="s">
+        <v>206</v>
+      </c>
+      <c r="B232" t="s">
+        <v>223</v>
+      </c>
+      <c r="C232">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A233" t="s">
+        <v>206</v>
+      </c>
+      <c r="B233" t="s">
+        <v>224</v>
+      </c>
+      <c r="C233">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A234" t="s">
+        <v>206</v>
+      </c>
+      <c r="B234" t="s">
+        <v>225</v>
+      </c>
+      <c r="C234">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A235" t="s">
+        <v>206</v>
+      </c>
+      <c r="B235" t="s">
+        <v>226</v>
+      </c>
+      <c r="C235">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A236" t="s">
+        <v>206</v>
+      </c>
+      <c r="B236" t="s">
+        <v>260</v>
+      </c>
+      <c r="C236">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A237" t="s">
+        <v>206</v>
+      </c>
+      <c r="B237" t="s">
+        <v>261</v>
+      </c>
+      <c r="C237">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A238" t="s">
+        <v>206</v>
+      </c>
+      <c r="B238" t="s">
+        <v>264</v>
+      </c>
+      <c r="C238">
+        <v>0.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>